<commit_message>
work on farr 1 day extended example
</commit_message>
<xml_diff>
--- a/day_1_manual/Detailed day 1 course outline.xlsx
+++ b/day_1_manual/Detailed day 1 course outline.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\Writing\teaching\Farr_Institute\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\farr_training\day_1_manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9612"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9612"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$98</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -635,6 +638,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -642,6 +660,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -656,29 +677,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -960,15 +963,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
     <col min="2" max="2" width="46.109375" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
   </cols>
@@ -988,7 +994,7 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="18" t="s">
         <v>89</v>
       </c>
       <c r="C2" s="1"/>
@@ -997,21 +1003,21 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="20" t="s">
         <v>156</v>
       </c>
       <c r="C5" s="3"/>
@@ -1020,21 +1026,21 @@
       <c r="A6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="23" t="s">
         <v>100</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1045,7 +1051,7 @@
       <c r="A9" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="5" t="s">
         <v>152</v>
       </c>
@@ -1054,7 +1060,7 @@
       <c r="A10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="5" t="s">
         <v>154</v>
       </c>
@@ -1063,7 +1069,7 @@
       <c r="A11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="5" t="s">
         <v>155</v>
       </c>
@@ -1072,7 +1078,7 @@
       <c r="A12" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="5" t="s">
         <v>144</v>
       </c>
@@ -1081,7 +1087,7 @@
       <c r="A13" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="18"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="5" t="s">
         <v>145</v>
       </c>
@@ -1090,7 +1096,7 @@
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="5" t="s">
         <v>153</v>
       </c>
@@ -1099,7 +1105,7 @@
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="5" t="s">
         <v>146</v>
       </c>
@@ -1108,7 +1114,7 @@
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="5" t="s">
         <v>147</v>
       </c>
@@ -1117,7 +1123,7 @@
       <c r="A17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="5" t="s">
         <v>148</v>
       </c>
@@ -1126,7 +1132,7 @@
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="18"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="5" t="s">
         <v>150</v>
       </c>
@@ -1135,7 +1141,7 @@
       <c r="A19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="30"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="14" t="s">
         <v>149</v>
       </c>
@@ -1144,7 +1150,7 @@
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="21" t="s">
         <v>101</v>
       </c>
       <c r="C20" s="1"/>
@@ -1153,42 +1159,42 @@
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="23" t="s">
         <v>102</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1199,7 +1205,7 @@
       <c r="A27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="5" t="s">
         <v>107</v>
       </c>
@@ -1208,7 +1214,7 @@
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="18"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="5" t="s">
         <v>108</v>
       </c>
@@ -1217,7 +1223,7 @@
       <c r="A29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="18"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="5" t="s">
         <v>109</v>
       </c>
@@ -1226,7 +1232,7 @@
       <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="18"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="5" t="s">
         <v>110</v>
       </c>
@@ -1235,7 +1241,7 @@
       <c r="A31" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="18"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="5" t="s">
         <v>111</v>
       </c>
@@ -1244,7 +1250,7 @@
       <c r="A32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="18"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="5" t="s">
         <v>112</v>
       </c>
@@ -1253,7 +1259,7 @@
       <c r="A33" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="18"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="5" t="s">
         <v>112</v>
       </c>
@@ -1262,7 +1268,7 @@
       <c r="A34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="30"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="14" t="s">
         <v>113</v>
       </c>
@@ -1271,7 +1277,7 @@
       <c r="A35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="16" t="s">
         <v>104</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -1282,7 +1288,7 @@
       <c r="A36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="23"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="4" t="s">
         <v>114</v>
       </c>
@@ -1291,7 +1297,7 @@
       <c r="A37" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="23"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="4" t="s">
         <v>115</v>
       </c>
@@ -1300,7 +1306,7 @@
       <c r="A38" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="23"/>
+      <c r="B38" s="16"/>
       <c r="C38" s="4" t="s">
         <v>116</v>
       </c>
@@ -1309,7 +1315,7 @@
       <c r="A39" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="23"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="4" t="s">
         <v>117</v>
       </c>
@@ -1318,7 +1324,7 @@
       <c r="A40" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="23"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="4" t="s">
         <v>118</v>
       </c>
@@ -1327,7 +1333,7 @@
       <c r="A41" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="23"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="4" t="s">
         <v>119</v>
       </c>
@@ -1336,7 +1342,7 @@
       <c r="A42" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="23"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="4" t="s">
         <v>120</v>
       </c>
@@ -1345,7 +1351,7 @@
       <c r="A43" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="24"/>
+      <c r="B43" s="17"/>
       <c r="C43" s="13" t="s">
         <v>120</v>
       </c>
@@ -1354,7 +1360,7 @@
       <c r="A44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="21" t="s">
         <v>105</v>
       </c>
       <c r="C44" s="1"/>
@@ -1363,84 +1369,84 @@
       <c r="A45" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="16"/>
+      <c r="B45" s="21"/>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="16"/>
+      <c r="B46" s="21"/>
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="16"/>
+      <c r="B47" s="21"/>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="16"/>
+      <c r="B48" s="21"/>
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="16"/>
+      <c r="B49" s="21"/>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="16"/>
+      <c r="B50" s="21"/>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="16"/>
+      <c r="B51" s="21"/>
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="16"/>
+      <c r="B52" s="21"/>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="16"/>
+      <c r="B53" s="21"/>
       <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="16"/>
+      <c r="B54" s="21"/>
       <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B55" s="17"/>
+      <c r="B55" s="22"/>
       <c r="C55" s="12"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="23" t="s">
         <v>137</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -1451,7 +1457,7 @@
       <c r="A57" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="18"/>
+      <c r="B57" s="23"/>
       <c r="C57" s="5" t="s">
         <v>122</v>
       </c>
@@ -1460,7 +1466,7 @@
       <c r="A58" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B58" s="18"/>
+      <c r="B58" s="23"/>
       <c r="C58" s="5" t="s">
         <v>123</v>
       </c>
@@ -1469,7 +1475,7 @@
       <c r="A59" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="18"/>
+      <c r="B59" s="23"/>
       <c r="C59" s="5" t="s">
         <v>123</v>
       </c>
@@ -1478,7 +1484,7 @@
       <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="18"/>
+      <c r="B60" s="23"/>
       <c r="C60" s="5" t="s">
         <v>124</v>
       </c>
@@ -1487,7 +1493,7 @@
       <c r="A61" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B61" s="18"/>
+      <c r="B61" s="23"/>
       <c r="C61" s="5" t="s">
         <v>125</v>
       </c>
@@ -1496,7 +1502,7 @@
       <c r="A62" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="18"/>
+      <c r="B62" s="23"/>
       <c r="C62" s="5" t="s">
         <v>125</v>
       </c>
@@ -1505,7 +1511,7 @@
       <c r="A63" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="18"/>
+      <c r="B63" s="23"/>
       <c r="C63" s="5" t="s">
         <v>126</v>
       </c>
@@ -1514,7 +1520,7 @@
       <c r="A64" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B64" s="18"/>
+      <c r="B64" s="23"/>
       <c r="C64" s="5" t="s">
         <v>126</v>
       </c>
@@ -1523,7 +1529,7 @@
       <c r="A65" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="18"/>
+      <c r="B65" s="23"/>
       <c r="C65" s="5" t="s">
         <v>127</v>
       </c>
@@ -1532,7 +1538,7 @@
       <c r="A66" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="18"/>
+      <c r="B66" s="23"/>
       <c r="C66" s="5" t="s">
         <v>127</v>
       </c>
@@ -1541,7 +1547,7 @@
       <c r="A67" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="18"/>
+      <c r="B67" s="23"/>
       <c r="C67" s="5" t="s">
         <v>128</v>
       </c>
@@ -1550,7 +1556,7 @@
       <c r="A68" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="18"/>
+      <c r="B68" s="23"/>
       <c r="C68" s="5" t="s">
         <v>128</v>
       </c>
@@ -1559,7 +1565,7 @@
       <c r="A69" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="18"/>
+      <c r="B69" s="23"/>
       <c r="C69" s="5" t="s">
         <v>129</v>
       </c>
@@ -1568,7 +1574,7 @@
       <c r="A70" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B70" s="18"/>
+      <c r="B70" s="23"/>
       <c r="C70" s="5" t="s">
         <v>130</v>
       </c>
@@ -1577,7 +1583,7 @@
       <c r="A71" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B71" s="18"/>
+      <c r="B71" s="23"/>
       <c r="C71" s="5" t="s">
         <v>131</v>
       </c>
@@ -1586,7 +1592,7 @@
       <c r="A72" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B72" s="18"/>
+      <c r="B72" s="23"/>
       <c r="C72" s="5" t="s">
         <v>132</v>
       </c>
@@ -1595,7 +1601,7 @@
       <c r="A73" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="18"/>
+      <c r="B73" s="23"/>
       <c r="C73" s="5" t="s">
         <v>133</v>
       </c>
@@ -1604,7 +1610,7 @@
       <c r="A74" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B74" s="18"/>
+      <c r="B74" s="23"/>
       <c r="C74" s="5" t="s">
         <v>134</v>
       </c>
@@ -1613,7 +1619,7 @@
       <c r="A75" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B75" s="18"/>
+      <c r="B75" s="23"/>
       <c r="C75" s="5" t="s">
         <v>135</v>
       </c>
@@ -1622,7 +1628,7 @@
       <c r="A76" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B76" s="18"/>
+      <c r="B76" s="23"/>
       <c r="C76" s="5" t="s">
         <v>135</v>
       </c>
@@ -1631,7 +1637,7 @@
       <c r="A77" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B77" s="18"/>
+      <c r="B77" s="23"/>
       <c r="C77" s="5" t="s">
         <v>135</v>
       </c>
@@ -1640,7 +1646,7 @@
       <c r="A78" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B78" s="18"/>
+      <c r="B78" s="23"/>
       <c r="C78" s="5" t="s">
         <v>136</v>
       </c>
@@ -1649,7 +1655,7 @@
       <c r="A79" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B79" s="19"/>
+      <c r="B79" s="25"/>
       <c r="C79" s="9" t="s">
         <v>136</v>
       </c>
@@ -1658,7 +1664,7 @@
       <c r="A80" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="26" t="s">
         <v>138</v>
       </c>
       <c r="C80" s="8" t="s">
@@ -1669,7 +1675,7 @@
       <c r="A81" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B81" s="20"/>
+      <c r="B81" s="26"/>
       <c r="C81" s="8" t="s">
         <v>138</v>
       </c>
@@ -1678,7 +1684,7 @@
       <c r="A82" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B82" s="21"/>
+      <c r="B82" s="27"/>
       <c r="C82" s="11" t="s">
         <v>138</v>
       </c>
@@ -1687,7 +1693,7 @@
       <c r="A83" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B83" s="22" t="s">
+      <c r="B83" s="28" t="s">
         <v>139</v>
       </c>
       <c r="C83" s="15" t="s">
@@ -1698,7 +1704,7 @@
       <c r="A84" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B84" s="23"/>
+      <c r="B84" s="16"/>
       <c r="C84" s="4" t="s">
         <v>139</v>
       </c>
@@ -1707,7 +1713,7 @@
       <c r="A85" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B85" s="23"/>
+      <c r="B85" s="16"/>
       <c r="C85" s="4" t="s">
         <v>139</v>
       </c>
@@ -1716,7 +1722,7 @@
       <c r="A86" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B86" s="23"/>
+      <c r="B86" s="16"/>
       <c r="C86" s="4" t="s">
         <v>139</v>
       </c>
@@ -1725,7 +1731,7 @@
       <c r="A87" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B87" s="23"/>
+      <c r="B87" s="16"/>
       <c r="C87" s="4" t="s">
         <v>139</v>
       </c>
@@ -1734,7 +1740,7 @@
       <c r="A88" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B88" s="23"/>
+      <c r="B88" s="16"/>
       <c r="C88" s="4" t="s">
         <v>139</v>
       </c>
@@ -1743,7 +1749,7 @@
       <c r="A89" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B89" s="23"/>
+      <c r="B89" s="16"/>
       <c r="C89" s="4" t="s">
         <v>139</v>
       </c>
@@ -1752,7 +1758,7 @@
       <c r="A90" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B90" s="23"/>
+      <c r="B90" s="16"/>
       <c r="C90" s="4" t="s">
         <v>139</v>
       </c>
@@ -1761,7 +1767,7 @@
       <c r="A91" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B91" s="23"/>
+      <c r="B91" s="16"/>
       <c r="C91" s="4" t="s">
         <v>139</v>
       </c>
@@ -1770,7 +1776,7 @@
       <c r="A92" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B92" s="23"/>
+      <c r="B92" s="16"/>
       <c r="C92" s="4" t="s">
         <v>139</v>
       </c>
@@ -1779,7 +1785,7 @@
       <c r="A93" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B93" s="23"/>
+      <c r="B93" s="16"/>
       <c r="C93" s="4" t="s">
         <v>139</v>
       </c>
@@ -1788,7 +1794,7 @@
       <c r="A94" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B94" s="24"/>
+      <c r="B94" s="17"/>
       <c r="C94" s="13" t="s">
         <v>139</v>
       </c>
@@ -1797,7 +1803,7 @@
       <c r="A95" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B95" s="25" t="s">
+      <c r="B95" s="29" t="s">
         <v>140</v>
       </c>
       <c r="C95" s="6" t="s">
@@ -1808,7 +1814,7 @@
       <c r="A96" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B96" s="25"/>
+      <c r="B96" s="29"/>
       <c r="C96" s="6" t="s">
         <v>141</v>
       </c>
@@ -1817,7 +1823,7 @@
       <c r="A97" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B97" s="25"/>
+      <c r="B97" s="29"/>
       <c r="C97" s="6" t="s">
         <v>142</v>
       </c>
@@ -1826,26 +1832,26 @@
       <c r="A98" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B98" s="26"/>
+      <c r="B98" s="30"/>
       <c r="C98" s="10" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B44:B55"/>
+    <mergeCell ref="B56:B79"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="B83:B94"/>
+    <mergeCell ref="B95:B98"/>
     <mergeCell ref="B35:B43"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B19"/>
     <mergeCell ref="B20:B25"/>
     <mergeCell ref="B26:B34"/>
-    <mergeCell ref="B44:B55"/>
-    <mergeCell ref="B56:B79"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="B83:B94"/>
-    <mergeCell ref="B95:B98"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="94" fitToHeight="12" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>